<commit_message>
added 33 label to the datas
</commit_message>
<xml_diff>
--- a/Notebooks/12_ICR-Test_letter-recognition-on-full-page_tagli_etichettati.xlsx
+++ b/Notebooks/12_ICR-Test_letter-recognition-on-full-page_tagli_etichettati.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\In-Codice-Ratio-OCR-with-CNN\Notebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documenti\Università\II Anno\Agiw\CNN\Notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="30">
   <si>
     <t>o</t>
   </si>
@@ -99,6 +99,21 @@
   </si>
   <si>
     <t>il taglio non è pulitissimo, la 1 e la 4 riconoscono la s, ma danno un ranking più alto alla s_mediana rispetto alla s_alta</t>
+  </si>
+  <si>
+    <t>èalksjojlk</t>
+  </si>
+  <si>
+    <t>pezzo di d mediana</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>in tutte le pipeline è la seconda scelta</t>
   </si>
 </sst>
 </file>
@@ -151,9 +166,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Cella collegata" xfId="1" builtinId="24"/>
@@ -469,13 +485,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G104"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -1436,7 +1455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>1608</v>
@@ -1451,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>1609</v>
@@ -1466,7 +1485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" ref="A67:A100" si="1">A66+1</f>
         <v>1610</v>
@@ -1481,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>1611</v>
@@ -1496,7 +1515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>1612</v>
@@ -1517,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>1613</v>
@@ -1538,160 +1557,376 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>1614</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1</v>
+      </c>
+      <c r="G71" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>1615</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>1616</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+      <c r="G73" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>1617</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>1618</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>1619</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>1620</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>1621</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1</v>
+      </c>
+      <c r="F78" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>1622</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>1623</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>1624</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
+        <v>1</v>
+      </c>
+      <c r="F81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>1625</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>1626</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>1</v>
+      </c>
+      <c r="F83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>1627</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>2</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1</v>
+      </c>
+      <c r="E84" t="s">
+        <v>1</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>1628</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>1629</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>1</v>
+      </c>
+      <c r="F86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>1630</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>27</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>1</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>1631</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>2</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1</v>
+      </c>
+      <c r="E88" t="s">
+        <v>1</v>
+      </c>
+      <c r="F88" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>1632</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1</v>
+      </c>
+      <c r="F89" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>1633</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>28</v>
+      </c>
+      <c r="G90" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>1634</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>1635</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1</v>
+      </c>
+      <c r="F92" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>1636</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>2</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>1637</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s">
+        <v>1</v>
+      </c>
+      <c r="F94" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>1638</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>1639</v>
+      </c>
+      <c r="B96" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -1699,27 +1934,71 @@
         <f t="shared" si="1"/>
         <v>1640</v>
       </c>
+      <c r="B97" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>1</v>
+      </c>
+      <c r="E97" t="s">
+        <v>1</v>
+      </c>
+      <c r="F97" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>1641</v>
       </c>
+      <c r="B98" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1</v>
+      </c>
+      <c r="F98" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>1642</v>
       </c>
+      <c r="B99" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1</v>
+      </c>
+      <c r="F99" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>1643</v>
       </c>
+      <c r="B100" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s">
+        <v>1</v>
+      </c>
+      <c r="F100" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="101" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="1"/>
+      <c r="A101" s="1">
+        <v>1644</v>
+      </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -1727,42 +2006,129 @@
       <c r="F101" s="1"/>
     </row>
     <row r="102" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="A102">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1646</v>
+      </c>
+      <c r="B103" t="s">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1</v>
+      </c>
+      <c r="D103" t="s">
+        <v>1</v>
+      </c>
+      <c r="E103" t="s">
+        <v>1</v>
+      </c>
+      <c r="F103" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>1647</v>
+      </c>
+      <c r="B104" t="s">
+        <v>2</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1</v>
+      </c>
+      <c r="D104" t="s">
+        <v>1</v>
+      </c>
+      <c r="E104" t="s">
+        <v>1</v>
+      </c>
+      <c r="F104" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>1648</v>
+      </c>
+      <c r="B105" t="s">
+        <v>2</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1</v>
+      </c>
+      <c r="E105" t="s">
+        <v>1</v>
+      </c>
+      <c r="F105" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>1649</v>
+      </c>
+      <c r="B106" t="s">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s">
+        <v>1</v>
+      </c>
+      <c r="F106" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1650</v>
+      </c>
+      <c r="B107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>10</v>
       </c>
-      <c r="B102">
-        <f>COUNTA(C1:C100)</f>
+      <c r="B111">
+        <f>COUNTA(C1:C107)</f>
+        <v>24</v>
+      </c>
+      <c r="C111">
+        <f>COUNTA(D1:D107)</f>
+        <v>76</v>
+      </c>
+      <c r="D111">
+        <f>COUNTA(E1:E107)</f>
+        <v>24</v>
+      </c>
+      <c r="E111">
+        <f>COUNTA(F1:F107)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>12</v>
+      </c>
+      <c r="C113" t="s">
         <v>14</v>
       </c>
-      <c r="C102">
-        <f>COUNTA(D1:D100)</f>
-        <v>52</v>
-      </c>
-      <c r="D102">
-        <f>COUNTA(E1:E100)</f>
-        <v>14</v>
-      </c>
-      <c r="E102">
-        <f>COUNTA(F1:F100)</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
+      <c r="D113" t="s">
         <v>12</v>
       </c>
-      <c r="C104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D104" t="s">
-        <v>12</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="E113" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>